<commit_message>
Pushing results of overnight test
</commit_message>
<xml_diff>
--- a/Scales/Scale Cailbration.xlsx
+++ b/Scales/Scale Cailbration.xlsx
@@ -1,35 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donal\Desktop\All Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcoon\Documents\GitHub\Modified-Energy-Cascade\Scales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E2E9E4-D8A1-415E-9AE8-85CACC6259C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC06AF5C-3DBF-41AF-8733-C364612184FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{EAD02111-A838-4B8A-8C65-4F4395CBA700}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{EAD02111-A838-4B8A-8C65-4F4395CBA700}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -420,16 +409,16 @@
   <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="9.7265625" customWidth="1"/>
-    <col min="8" max="8" width="10.26953125" customWidth="1"/>
+    <col min="3" max="3" width="9.77734375" customWidth="1"/>
+    <col min="8" max="8" width="10.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -441,7 +430,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -461,7 +450,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>22784</v>
       </c>
@@ -483,7 +472,7 @@
         <v>-467.67477488641515</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>22747</v>
       </c>
@@ -498,14 +487,14 @@
         <v>21359</v>
       </c>
       <c r="G4">
-        <v>46.593649999999997</v>
+        <v>45.593649999999997</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H8" si="1">-F4/G4</f>
-        <v>-458.41010523966253</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+        <v>-468.46435852361026</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>22731</v>
       </c>
@@ -520,14 +509,14 @@
         <v>21327</v>
       </c>
       <c r="G5">
-        <v>47.593649999999997</v>
+        <v>45.593649999999997</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>-448.10599733367798</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>-467.76250640165904</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>22768</v>
       </c>
@@ -542,14 +531,14 @@
         <v>21367</v>
       </c>
       <c r="G6">
-        <v>48.593649999999997</v>
+        <v>45.593649999999997</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>-439.70765727620795</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+        <v>-468.63982155409803</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>22754</v>
       </c>
@@ -564,14 +553,14 @@
         <v>21380</v>
       </c>
       <c r="G7">
-        <v>49.593649999999997</v>
+        <v>45.593649999999997</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>-431.10357878478396</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+        <v>-468.92494897864071</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>22715</v>
       </c>
@@ -586,14 +575,14 @@
         <v>21314</v>
       </c>
       <c r="G8">
-        <v>50.593649999999997</v>
+        <v>45.593649999999997</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>-421.27816435461767</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+        <v>-467.47737897711636</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -605,10 +594,11 @@
         <v>6</v>
       </c>
       <c r="H9">
-        <v>-464.66320000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+        <f>AVERAGE(H3:H8)</f>
+        <v>-468.15729822025651</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -622,7 +612,7 @@
         <v>-464</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -634,7 +624,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -654,7 +644,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>22739</v>
       </c>
@@ -673,7 +663,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>22712</v>
       </c>
@@ -692,7 +682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>22707</v>
       </c>
@@ -711,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>22707</v>
       </c>
@@ -730,7 +720,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>22371</v>
       </c>
@@ -749,7 +739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>22757</v>
       </c>
@@ -768,7 +758,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -784,7 +774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
Moving  on to multiplexing the Scales
</commit_message>
<xml_diff>
--- a/Scales/Scale Cailbration.xlsx
+++ b/Scales/Scale Cailbration.xlsx
@@ -1,24 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dcoon\Documents\GitHub\Modified-Energy-Cascade\Scales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donal\Documents\GitHub\Modified-Energy-Cascade\Scales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC06AF5C-3DBF-41AF-8733-C364612184FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359BF9E1-7088-4D40-A4CE-B907D9429317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{EAD02111-A838-4B8A-8C65-4F4395CBA700}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{EAD02111-A838-4B8A-8C65-4F4395CBA700}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -408,17 +419,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B72FDE0-55F2-466B-A466-75B6AA6026B9}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="9.77734375" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -430,7 +441,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
     </row>
-    <row r="2" spans="1:8" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="14" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -450,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>22784</v>
       </c>
@@ -472,7 +483,7 @@
         <v>-467.67477488641515</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>22747</v>
       </c>
@@ -494,7 +505,7 @@
         <v>-468.46435852361026</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>22731</v>
       </c>
@@ -516,7 +527,7 @@
         <v>-467.76250640165904</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>22768</v>
       </c>
@@ -538,7 +549,7 @@
         <v>-468.63982155409803</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>22754</v>
       </c>
@@ -560,7 +571,7 @@
         <v>-468.92494897864071</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>22715</v>
       </c>
@@ -582,7 +593,7 @@
         <v>-467.47737897711636</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -598,7 +609,7 @@
         <v>-468.15729822025651</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -612,7 +623,7 @@
         <v>-464</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
@@ -624,7 +635,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -644,7 +655,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>22739</v>
       </c>
@@ -663,7 +674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>22712</v>
       </c>
@@ -682,7 +693,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>22707</v>
       </c>
@@ -701,7 +712,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>22707</v>
       </c>
@@ -720,7 +731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>22371</v>
       </c>
@@ -739,7 +750,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>22757</v>
       </c>
@@ -758,7 +769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>6</v>
       </c>
@@ -774,7 +785,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>5</v>
       </c>

</xml_diff>

<commit_message>
I think I solved the sobol output issue!!
</commit_message>
<xml_diff>
--- a/Scales/Scale Cailbration.xlsx
+++ b/Scales/Scale Cailbration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donal\Documents\GitHub\Modified-Energy-Cascade\Scales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{359BF9E1-7088-4D40-A4CE-B907D9429317}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640922D1-5CE1-4BB6-AE59-B5CF50E98792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="10170" xr2:uid="{EAD02111-A838-4B8A-8C65-4F4395CBA700}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" xr2:uid="{EAD02111-A838-4B8A-8C65-4F4395CBA700}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B72FDE0-55F2-466B-A466-75B6AA6026B9}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -666,12 +666,15 @@
         <f>-A14/B14</f>
         <v>-498.73173128275545</v>
       </c>
+      <c r="F14">
+        <v>10498</v>
+      </c>
       <c r="G14">
-        <v>45.593649999999997</v>
+        <v>22.761500000000002</v>
       </c>
       <c r="H14">
         <f>-F14/G14</f>
-        <v>0</v>
+        <v>-461.21740658568194</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -685,12 +688,15 @@
         <f t="shared" ref="C15:C19" si="2">-A15/B15</f>
         <v>-498.13954355485907</v>
       </c>
+      <c r="F15">
+        <v>10495</v>
+      </c>
       <c r="G15">
-        <v>46.593649999999997</v>
+        <v>22.761500000000002</v>
       </c>
       <c r="H15">
         <f t="shared" ref="H15:H19" si="3">-F15/G15</f>
-        <v>0</v>
+        <v>-461.08560507875137</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -704,12 +710,15 @@
         <f t="shared" si="2"/>
         <v>-498.02987916080423</v>
       </c>
+      <c r="F16">
+        <v>10484</v>
+      </c>
       <c r="G16">
-        <v>47.593649999999997</v>
+        <v>22.761500000000002</v>
       </c>
       <c r="H16">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-460.60233288667263</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -723,12 +732,15 @@
         <f t="shared" si="2"/>
         <v>-498.02987916080423</v>
       </c>
+      <c r="F17">
+        <v>10474</v>
+      </c>
       <c r="G17">
-        <v>48.593649999999997</v>
+        <v>22.761500000000002</v>
       </c>
       <c r="H17">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-460.16299453023743</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -742,12 +754,15 @@
         <f t="shared" si="2"/>
         <v>-490.66043188031671</v>
       </c>
+      <c r="F18">
+        <v>10507</v>
+      </c>
       <c r="G18">
-        <v>49.593649999999997</v>
+        <v>22.761500000000002</v>
       </c>
       <c r="H18">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-461.6128111064736</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -761,12 +776,15 @@
         <f t="shared" si="2"/>
         <v>-499.12652310135297</v>
       </c>
+      <c r="F19">
+        <v>10428</v>
+      </c>
       <c r="G19">
-        <v>50.593649999999997</v>
+        <v>22.761500000000002</v>
       </c>
       <c r="H19">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>-458.14203809063548</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -782,7 +800,7 @@
       </c>
       <c r="H20">
         <f>AVERAGE(H14:H19)</f>
-        <v>0</v>
+        <v>-460.47053137974217</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -794,9 +812,6 @@
       </c>
       <c r="F21" t="s">
         <v>5</v>
-      </c>
-      <c r="H21">
-        <v>-498</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Got single scale to work off mosfet
</commit_message>
<xml_diff>
--- a/Scales/Scale Cailbration.xlsx
+++ b/Scales/Scale Cailbration.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\donal\Documents\GitHub\Modified-Energy-Cascade\Scales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640922D1-5CE1-4BB6-AE59-B5CF50E98792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0625FDF-6A67-4FE4-8462-CFCE0C75AF6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14400" windowHeight="7270" xr2:uid="{EAD02111-A838-4B8A-8C65-4F4395CBA700}"/>
+    <workbookView xWindow="9930" yWindow="0" windowWidth="9360" windowHeight="10170" xr2:uid="{EAD02111-A838-4B8A-8C65-4F4395CBA700}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -419,8 +419,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B72FDE0-55F2-466B-A466-75B6AA6026B9}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -463,134 +463,134 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>22784</v>
+        <v>-47777</v>
       </c>
       <c r="B3">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C3">
         <f>-A3/B3</f>
-        <v>-499.71871082924929</v>
+        <v>471.17357001972385</v>
       </c>
       <c r="F3">
-        <v>21323</v>
+        <v>49996</v>
       </c>
       <c r="G3">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="H3">
         <f>-F3/G3</f>
-        <v>-467.67477488641515</v>
+        <v>-493.05719921104532</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>22747</v>
+        <v>-47767</v>
       </c>
       <c r="B4">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C4">
         <f t="shared" ref="C4:C8" si="0">-A4/B4</f>
-        <v>-498.90719431324322</v>
+        <v>471.0749506903353</v>
       </c>
       <c r="F4">
-        <v>21359</v>
+        <v>50065</v>
       </c>
       <c r="G4">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="H4">
         <f t="shared" ref="H4:H8" si="1">-F4/G4</f>
-        <v>-468.46435852361026</v>
+        <v>-493.7376725838264</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>22731</v>
+        <v>-47764</v>
       </c>
       <c r="B5">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C5">
         <f t="shared" si="0"/>
-        <v>-498.55626825226761</v>
+        <v>471.04536489151872</v>
       </c>
       <c r="F5">
-        <v>21327</v>
+        <v>50048</v>
       </c>
       <c r="G5">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="H5">
         <f t="shared" si="1"/>
-        <v>-467.76250640165904</v>
+        <v>-493.57001972386587</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>22768</v>
+        <v>-47746</v>
       </c>
       <c r="B6">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>-499.36778476827368</v>
+        <v>470.86785009861933</v>
       </c>
       <c r="F6">
-        <v>21367</v>
+        <v>49996</v>
       </c>
       <c r="G6">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="H6">
         <f t="shared" si="1"/>
-        <v>-468.63982155409803</v>
+        <v>-493.05719921104532</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>22754</v>
+        <v>-47728</v>
       </c>
       <c r="B7">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>-499.06072446492004</v>
+        <v>470.69033530571988</v>
       </c>
       <c r="F7">
-        <v>21380</v>
+        <v>50046</v>
       </c>
       <c r="G7">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="H7">
         <f t="shared" si="1"/>
-        <v>-468.92494897864071</v>
+        <v>-493.55029585798815</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>22715</v>
+        <v>-47767</v>
       </c>
       <c r="B8">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>-498.205342191292</v>
+        <v>471.0749506903353</v>
       </c>
       <c r="F8">
-        <v>21314</v>
+        <v>49878</v>
       </c>
       <c r="G8">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="H8">
         <f t="shared" si="1"/>
-        <v>-467.47737897711636</v>
+        <v>-491.89349112426032</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -599,28 +599,22 @@
       </c>
       <c r="C9">
         <f>AVERAGE(C3:C8)</f>
-        <v>-498.96933746987429</v>
+        <v>470.98783694937543</v>
       </c>
       <c r="F9" t="s">
         <v>6</v>
       </c>
       <c r="H9">
         <f>AVERAGE(H3:H8)</f>
-        <v>-468.15729822025651</v>
+        <v>-493.14431295200524</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
-      <c r="C10">
-        <v>-498</v>
-      </c>
       <c r="F10" t="s">
         <v>5</v>
-      </c>
-      <c r="H10">
-        <v>-464</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -657,134 +651,134 @@
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>22739</v>
+        <v>-47621</v>
       </c>
       <c r="B14">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C14">
         <f>-A14/B14</f>
-        <v>-498.73173128275545</v>
+        <v>469.63510848126231</v>
       </c>
       <c r="F14">
-        <v>10498</v>
+        <v>-52090</v>
       </c>
       <c r="G14">
-        <v>22.761500000000002</v>
+        <v>101.4</v>
       </c>
       <c r="H14">
         <f>-F14/G14</f>
-        <v>-461.21740658568194</v>
+        <v>513.70808678500987</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>22712</v>
+        <v>-47316</v>
       </c>
       <c r="B15">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C15">
         <f t="shared" ref="C15:C19" si="2">-A15/B15</f>
-        <v>-498.13954355485907</v>
+        <v>466.62721893491124</v>
       </c>
       <c r="F15">
-        <v>10495</v>
+        <v>-50224</v>
       </c>
       <c r="G15">
-        <v>22.761500000000002</v>
+        <v>101.4</v>
       </c>
       <c r="H15">
         <f t="shared" ref="H15:H19" si="3">-F15/G15</f>
-        <v>-461.08560507875137</v>
+        <v>495.30571992110453</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>22707</v>
+        <v>-47268</v>
       </c>
       <c r="B16">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C16">
         <f t="shared" si="2"/>
-        <v>-498.02987916080423</v>
+        <v>466.15384615384613</v>
       </c>
       <c r="F16">
-        <v>10484</v>
+        <v>-50201</v>
       </c>
       <c r="G16">
-        <v>22.761500000000002</v>
+        <v>101.4</v>
       </c>
       <c r="H16">
         <f t="shared" si="3"/>
-        <v>-460.60233288667263</v>
+        <v>495.07889546351083</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>22707</v>
+        <v>-47288</v>
       </c>
       <c r="B17">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C17">
         <f t="shared" si="2"/>
-        <v>-498.02987916080423</v>
+        <v>466.35108481262324</v>
       </c>
       <c r="F17">
-        <v>10474</v>
+        <v>-50189</v>
       </c>
       <c r="G17">
-        <v>22.761500000000002</v>
+        <v>101.4</v>
       </c>
       <c r="H17">
         <f t="shared" si="3"/>
-        <v>-460.16299453023743</v>
+        <v>494.96055226824456</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>22371</v>
+        <v>-47322</v>
       </c>
       <c r="B18">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C18">
         <f t="shared" si="2"/>
-        <v>-490.66043188031671</v>
+        <v>466.68639053254435</v>
       </c>
       <c r="F18">
-        <v>10507</v>
+        <v>-50169</v>
       </c>
       <c r="G18">
-        <v>22.761500000000002</v>
+        <v>101.4</v>
       </c>
       <c r="H18">
         <f t="shared" si="3"/>
-        <v>-461.6128111064736</v>
+        <v>494.76331360946745</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>22757</v>
+        <v>-47300</v>
       </c>
       <c r="B19">
-        <v>45.593649999999997</v>
+        <v>101.4</v>
       </c>
       <c r="C19">
         <f t="shared" si="2"/>
-        <v>-499.12652310135297</v>
+        <v>466.46942800788952</v>
       </c>
       <c r="F19">
-        <v>10428</v>
+        <v>-50166</v>
       </c>
       <c r="G19">
-        <v>22.761500000000002</v>
+        <v>101.4</v>
       </c>
       <c r="H19">
         <f t="shared" si="3"/>
-        <v>-458.14203809063548</v>
+        <v>494.73372781065086</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -793,22 +787,19 @@
       </c>
       <c r="C20">
         <f>AVERAGE(C14:C19)</f>
-        <v>-497.1196646901488</v>
+        <v>466.9871794871795</v>
       </c>
       <c r="F20" t="s">
         <v>6</v>
       </c>
       <c r="H20">
         <f>AVERAGE(H14:H19)</f>
-        <v>-460.47053137974217</v>
+        <v>498.09171597633139</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>5</v>
-      </c>
-      <c r="C21">
-        <v>-498</v>
       </c>
       <c r="F21" t="s">
         <v>5</v>

</xml_diff>